<commit_message>
Updated id and ax proj int
</commit_message>
<xml_diff>
--- a/Fix/fix cur. 19.xlsx
+++ b/Fix/fix cur. 19.xlsx
@@ -43,9 +43,6 @@
     <t>ax</t>
   </si>
   <si>
-    <t>ib</t>
-  </si>
-  <si>
     <t>mature</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>24106000098528</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -429,9 +429,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -806,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -848,13 +845,13 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="2"/>
@@ -902,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>7</v>
@@ -919,7 +916,7 @@
         <v>8062.666666666667</v>
       </c>
       <c r="J3" s="42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3" s="39"/>
       <c r="L3" s="43"/>
@@ -962,7 +959,7 @@
         <v>3442</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="11"/>
@@ -1003,7 +1000,7 @@
         <v>1209</v>
       </c>
       <c r="J5" s="55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="53"/>
       <c r="L5" s="56"/>
@@ -1072,7 +1069,7 @@
         <v>10215</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" s="22"/>
       <c r="L7" s="24"/>
@@ -1113,7 +1110,7 @@
         <v>4830</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="11"/>
@@ -1154,7 +1151,7 @@
         <v>3425</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="11"/>
@@ -1186,16 +1183,16 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="21">
-        <v>41818</v>
+        <v>41816</v>
       </c>
       <c r="H10" s="21">
-        <v>42549</v>
-      </c>
-      <c r="I10" s="60">
-        <v>2200</v>
+        <v>42547</v>
+      </c>
+      <c r="I10" s="30">
+        <v>2309</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="11"/>
@@ -1246,13 +1243,13 @@
         <v>9.6</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="15">
@@ -1265,7 +1262,7 @@
         <v>3175</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="11"/>
@@ -1287,13 +1284,13 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="15">
@@ -1306,7 +1303,7 @@
         <v>10125</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="11"/>
@@ -1328,13 +1325,13 @@
         <v>9.6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="15">
@@ -1347,7 +1344,7 @@
         <v>3175</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="11"/>
@@ -1404,7 +1401,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="15">
@@ -1417,7 +1414,7 @@
         <v>3353</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="11"/>
@@ -1445,7 +1442,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="15">
@@ -1458,7 +1455,7 @@
         <v>1871</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="11"/>
@@ -1480,13 +1477,13 @@
         <v>9.43</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="15">
@@ -1499,7 +1496,7 @@
         <v>2322</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="11"/>
@@ -1521,13 +1518,13 @@
         <v>9.43</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="15">
@@ -1540,7 +1537,7 @@
         <v>9531</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="11"/>
@@ -1562,13 +1559,13 @@
         <v>9.43</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="15">
@@ -1581,7 +1578,7 @@
         <v>2843</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="11"/>
@@ -1638,7 +1635,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="15">
@@ -1651,7 +1648,7 @@
         <v>2000</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="11"/>
@@ -1673,13 +1670,13 @@
         <v>9.75</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="5">
@@ -1692,7 +1689,7 @@
         <v>3169</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="4"/>
@@ -1720,7 +1717,7 @@
         <v>6</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="5">
@@ -1733,7 +1730,7 @@
         <v>2803</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
@@ -1761,7 +1758,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="5">
@@ -1774,7 +1771,7 @@
         <v>4672</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="4"/>
@@ -1802,7 +1799,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="29">
@@ -1815,7 +1812,7 @@
         <v>2559</v>
       </c>
       <c r="J26" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K26" s="28"/>
       <c r="L26" s="32"/>
@@ -1843,7 +1840,7 @@
         <v>6</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="5">
@@ -1856,7 +1853,7 @@
         <v>3656</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="4"/>
@@ -1881,10 +1878,10 @@
         <v>60</v>
       </c>
       <c r="D28" s="45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E28" s="45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="45"/>
       <c r="G28" s="46">
@@ -1898,7 +1895,7 @@
         <v>375</v>
       </c>
       <c r="J28" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K28" s="45"/>
       <c r="L28" s="48"/>
@@ -1966,7 +1963,7 @@
     </row>
     <row r="31" spans="1:21" ht="12.75" customHeight="1">
       <c r="A31" s="51">
-        <v>41844</v>
+        <v>41849</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="3"/>
@@ -1980,7 +1977,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="16">
         <f>SUM(I3:I27)</f>
-        <v>88637.666666666672</v>
+        <v>88746.666666666672</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>3</v>
@@ -2033,7 +2030,7 @@
         <v>17336</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="4"/>
@@ -2082,7 +2079,7 @@
       <c r="H35" s="4"/>
       <c r="I35" s="17">
         <f>I31+I33</f>
-        <v>105973.66666666667</v>
+        <v>106082.66666666667</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2165,7 +2162,7 @@
     </row>
     <row r="39" spans="1:21" ht="12.75" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="4">
         <v>250000</v>
@@ -2196,7 +2193,7 @@
     </row>
     <row r="40" spans="1:21" ht="12.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="4">
         <v>250000</v>
@@ -2227,19 +2224,19 @@
     </row>
     <row r="41" spans="1:21" ht="12.75" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="4">
         <v>250000</v>
       </c>
       <c r="C41" s="4">
-        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11)</f>
-        <v>216345</v>
+        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11) + (1331 + 3175 * 8)</f>
+        <v>243076</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4">
         <f t="shared" ref="E41:E43" si="0">B41-C41</f>
-        <v>33655</v>
+        <v>6924</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41">
@@ -2255,7 +2252,7 @@
       </c>
       <c r="J41" s="50">
         <f>C41+I41</f>
-        <v>246345</v>
+        <v>273076</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="4"/>
@@ -2271,19 +2268,19 @@
     </row>
     <row r="42" spans="1:21" ht="12.75" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="4">
         <v>250000</v>
       </c>
       <c r="C42" s="4">
-        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567</f>
-        <v>224022</v>
+        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567 + (2309 * 9)</f>
+        <v>244803</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4">
-        <f t="shared" si="0"/>
-        <v>25978</v>
+        <f>B42-C42</f>
+        <v>5197</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42">
@@ -2299,7 +2296,7 @@
       </c>
       <c r="J42" s="50">
         <f>C42+I42</f>
-        <v>245397</v>
+        <v>266178</v>
       </c>
       <c r="K42" s="3"/>
       <c r="L42" s="4"/>
@@ -2315,7 +2312,7 @@
     </row>
     <row r="43" spans="1:21" ht="12.75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" s="4">
         <v>250000</v>

</xml_diff>